<commit_message>
Alterações e Correções sugeridas
- Alteração da Visão Geral
- Alterações Requisitos e Descrição dos UC
- Alterações Especificações UC
- Melhorias nos Códigos e Interfaces
</commit_message>
<xml_diff>
--- a/Requisitos/Requisitos e Descrição dos Casos de Uso.xlsx
+++ b/Requisitos/Requisitos e Descrição dos Casos de Uso.xlsx
@@ -38,9 +38,6 @@
     <t>RE02</t>
   </si>
   <si>
-    <t>O usuário necessita se cadastrar para utilizar o sistema.</t>
-  </si>
-  <si>
     <t>Registrar Usuário</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>RE04</t>
   </si>
   <si>
-    <t>Enviar e-mail para o usuário contendo link para ativação do usuário</t>
-  </si>
-  <si>
     <t>Enviar e-mail de ativação</t>
   </si>
   <si>
@@ -107,21 +101,12 @@
     <t>DIRETOR</t>
   </si>
   <si>
-    <t>O recepcionista poderá fazer marcação, desmarcação, listagem de consultas</t>
-  </si>
-  <si>
     <t>Manter consulta</t>
   </si>
   <si>
-    <t>O recepcionista irá manter os pacientes.</t>
-  </si>
-  <si>
     <t>Manter paciente</t>
   </si>
   <si>
-    <t>RECEPCIONISTA</t>
-  </si>
-  <si>
     <t>RE12</t>
   </si>
   <si>
@@ -131,9 +116,6 @@
     <t>Manter consulta de encaixe</t>
   </si>
   <si>
-    <t>MEDICO</t>
-  </si>
-  <si>
     <t>REQUISITOS DO SISTEMA</t>
   </si>
   <si>
@@ -213,6 +195,24 @@
   </si>
   <si>
     <t>RE13</t>
+  </si>
+  <si>
+    <t>MEDICO/RECEPCIONISTA/DIRETOR</t>
+  </si>
+  <si>
+    <t>RECEPCIONISTA/MEDICO/DIRETOR</t>
+  </si>
+  <si>
+    <t>O diretor irá cadastrar o usuário no sistema.</t>
+  </si>
+  <si>
+    <t>Enviar e-mail para o usuário contendo link de ativação.</t>
+  </si>
+  <si>
+    <t>O usuário poderá fazer marcação, desmarcação, listagem de consultas, reagendamento</t>
+  </si>
+  <si>
+    <t>O usuário irá manter os pacientes.</t>
   </si>
 </sst>
 </file>
@@ -675,19 +675,19 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="82" customWidth="1"/>
     <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -712,7 +712,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -726,167 +726,167 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15" x14ac:dyDescent="0.25">
@@ -909,13 +909,13 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
     </row>
     <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
@@ -938,134 +938,134 @@
     </row>
     <row r="3" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>